<commit_message>
Added Kotireddy -- Health Insurance policy no
</commit_message>
<xml_diff>
--- a/Insurance_info.xlsx
+++ b/Insurance_info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\503151006\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AE24565-4F3E-4AB9-A68D-5B3334C65B6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9894CB7D-7A8D-4F7E-B57D-1DC7305304F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{B8F15854-CD7D-4830-9D06-B0799B8D4201}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="47">
   <si>
     <t>Name</t>
   </si>
@@ -135,9 +135,6 @@
   </si>
   <si>
     <t>Policy No</t>
-  </si>
-  <si>
-    <t>Note: Policy No will change Every Year(Renewal)</t>
   </si>
   <si>
     <t>Company Insurance</t>
@@ -174,6 +171,17 @@
   </si>
   <si>
     <t>Payment Till</t>
+  </si>
+  <si>
+    <t>Collegue</t>
+  </si>
+  <si>
+    <t>1-Point Contact -- Akbar(Manager) --9247678125
+2-Point Contact --Ahmed(Friend) -- 8341187866
+whatsApp Group -- Oscar Finance Family</t>
+  </si>
+  <si>
+    <t>Note: Policy No will change Every Year(Renewal) - we can do renewal 3  months before</t>
   </si>
 </sst>
 </file>
@@ -206,7 +214,7 @@
     </font>
     <font>
       <b/>
-      <sz val="22"/>
+      <sz val="16"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -239,7 +247,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -270,20 +278,9 @@
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
+      <bottom style="thin">
         <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -291,11 +288,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
@@ -306,40 +302,44 @@
     <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -655,10 +655,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5689222B-D505-40C9-8681-40BFCA167C6B}">
-  <dimension ref="A1:M18"/>
+  <dimension ref="A1:N18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -672,10 +672,11 @@
     <col min="8" max="9" width="20.90625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17.54296875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="25.26953125" customWidth="1"/>
-    <col min="13" max="13" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.1796875" customWidth="1"/>
+    <col min="14" max="14" width="42.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -701,63 +702,69 @@
         <v>28</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M1" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="N1" s="2" t="s">
+        <v>44</v>
+      </c>
     </row>
-    <row r="2" spans="1:13" ht="58" x14ac:dyDescent="0.35">
-      <c r="A2" s="13" t="s">
+    <row r="2" spans="1:14" ht="58" x14ac:dyDescent="0.35">
+      <c r="A2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="13">
+      <c r="C2" s="9">
         <v>79019827</v>
       </c>
-      <c r="D2" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="E2" s="15">
+      <c r="D2" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" s="10">
         <v>45696</v>
       </c>
-      <c r="F2" s="16" t="s">
+      <c r="F2" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="G2" s="17">
+      <c r="G2" s="12">
         <v>18002585881</v>
       </c>
-      <c r="H2" s="18" t="s">
+      <c r="H2" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="I2" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="J2" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="K2" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="L2" s="14" t="s">
+      <c r="I2" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="J2" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="M2" s="11">
+      <c r="K2" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="L2" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="M2" s="21">
         <v>45808</v>
       </c>
+      <c r="N2" s="15" t="s">
+        <v>45</v>
+      </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -767,51 +774,65 @@
       <c r="C3" s="1">
         <v>94776573</v>
       </c>
-      <c r="D3" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="E3" s="9">
+      <c r="D3" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" s="8">
         <v>46018</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H3" s="6" t="s">
         <v>30</v>
       </c>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="20" t="s">
-        <v>40</v>
+      <c r="K3" s="14"/>
+      <c r="L3" s="17" t="s">
+        <v>39</v>
       </c>
       <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="21" t="s">
-        <v>43</v>
+      <c r="C4" s="1">
+        <v>94978211</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="8">
+        <v>46020</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="I4" s="20" t="s">
+        <v>42</v>
       </c>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -827,43 +848,44 @@
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A8" s="4" t="s">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A8" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="G8" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="H8" s="4" t="s">
+      <c r="H8" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="I8" s="4" t="s">
+      <c r="I8" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="J8" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="K8" s="4" t="s">
+      <c r="J8" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="K8" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>2</v>
       </c>
@@ -882,23 +904,23 @@
       <c r="F9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G9" s="5" t="s">
+      <c r="G9" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="H9" s="8">
+      <c r="H9" s="7">
         <v>18002585881</v>
       </c>
-      <c r="I9" s="7" t="s">
+      <c r="I9" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="J9" s="12">
+      <c r="J9" s="18">
         <v>55153</v>
       </c>
-      <c r="K9" s="9">
+      <c r="K9" s="8">
         <v>58837</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
@@ -915,19 +937,19 @@
       <c r="F10" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G10" s="5" t="s">
+      <c r="G10" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="H10" s="6" t="s">
+      <c r="H10" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="I10" s="7" t="s">
+      <c r="I10" s="6" t="s">
         <v>30</v>
       </c>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
@@ -942,39 +964,39 @@
         <v>18</v>
       </c>
       <c r="F11" s="1"/>
-      <c r="G11" s="5" t="s">
+      <c r="G11" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="H11" s="6" t="s">
+      <c r="H11" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="I11" s="7" t="s">
+      <c r="I11" s="6" t="s">
         <v>30</v>
       </c>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A17" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="10"/>
+      <c r="A17" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" s="22"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="22"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A18" s="10"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="10"/>
+      <c r="A18" s="22"/>
+      <c r="B18" s="22"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -986,6 +1008,7 @@
     <hyperlink ref="I11" r:id="rId3" xr:uid="{EA158189-5734-4048-94B7-B5A33B660C07}"/>
     <hyperlink ref="H2" r:id="rId4" xr:uid="{60556C6A-0414-4B91-84BF-430D7F960C65}"/>
     <hyperlink ref="I9" r:id="rId5" xr:uid="{0F9D3D11-7051-4FB3-8A41-B2B147082FE1}"/>
+    <hyperlink ref="H4" r:id="rId6" xr:uid="{70887739-DA10-494B-83D0-7CEE48172100}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added -- Murali Office Insurance details
</commit_message>
<xml_diff>
--- a/Insurance_info.xlsx
+++ b/Insurance_info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\503151006\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9894CB7D-7A8D-4F7E-B57D-1DC7305304F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A28833A2-AD2B-4FFD-B513-EF2D3EC024E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{B8F15854-CD7D-4830-9D06-B0799B8D4201}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="50">
   <si>
     <t>Name</t>
   </si>
@@ -182,6 +182,16 @@
   </si>
   <si>
     <t>Note: Policy No will change Every Year(Renewal) - we can do renewal 3  months before</t>
+  </si>
+  <si>
+    <t>14900(Ctrl S)</t>
+  </si>
+  <si>
+    <t>universal sompo general insurance</t>
+  </si>
+  <si>
+    <t>Murali(USGI51340704)
+Rajalaxmi(USGI53042804)</t>
   </si>
 </sst>
 </file>
@@ -288,7 +298,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -317,15 +327,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -338,6 +344,15 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -657,8 +672,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5689222B-D505-40C9-8681-40BFCA167C6B}">
   <dimension ref="A1:N18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -730,7 +745,7 @@
       <c r="C2" s="9">
         <v>79019827</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="15" t="s">
         <v>36</v>
       </c>
       <c r="E2" s="10">
@@ -748,23 +763,23 @@
       <c r="I2" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="J2" s="15" t="s">
+      <c r="J2" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="K2" s="15" t="s">
+      <c r="K2" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="L2" s="16" t="s">
+      <c r="L2" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="M2" s="21">
+      <c r="M2" s="19">
         <v>45808</v>
       </c>
-      <c r="N2" s="15" t="s">
+      <c r="N2" s="14" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -774,7 +789,7 @@
       <c r="C3" s="1">
         <v>94776573</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="17" t="s">
         <v>36</v>
       </c>
       <c r="E3" s="8">
@@ -789,13 +804,21 @@
       <c r="H3" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="17" t="s">
+      <c r="I3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J3" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="K3" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="L3" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="M3" s="1"/>
+      <c r="M3" s="19">
+        <v>45878</v>
+      </c>
       <c r="N3" s="1"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
@@ -808,7 +831,7 @@
       <c r="C4" s="1">
         <v>94978211</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="17" t="s">
         <v>36</v>
       </c>
       <c r="E4" s="8">
@@ -823,7 +846,7 @@
       <c r="H4" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="I4" s="20" t="s">
+      <c r="I4" s="18" t="s">
         <v>42</v>
       </c>
       <c r="J4" s="1"/>
@@ -913,7 +936,7 @@
       <c r="I9" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="J9" s="18">
+      <c r="J9" s="16">
         <v>55153</v>
       </c>
       <c r="K9" s="8">
@@ -977,26 +1000,26 @@
       <c r="K11" s="1"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A17" s="22" t="s">
+      <c r="A17" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="B17" s="22"/>
-      <c r="C17" s="22"/>
-      <c r="D17" s="22"/>
-      <c r="E17" s="22"/>
-      <c r="F17" s="22"/>
-      <c r="G17" s="22"/>
-      <c r="H17" s="22"/>
+      <c r="B17" s="20"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="20"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A18" s="22"/>
-      <c r="B18" s="22"/>
-      <c r="C18" s="22"/>
-      <c r="D18" s="22"/>
-      <c r="E18" s="22"/>
-      <c r="F18" s="22"/>
-      <c r="G18" s="22"/>
-      <c r="H18" s="22"/>
+      <c r="A18" s="20"/>
+      <c r="B18" s="20"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Added Alekya kotireddy term insurance details
</commit_message>
<xml_diff>
--- a/Insurance_info.xlsx
+++ b/Insurance_info.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\503151006\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A28833A2-AD2B-4FFD-B513-EF2D3EC024E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E32F9CCA-74BC-4036-898F-40D461F92682}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{B8F15854-CD7D-4830-9D06-B0799B8D4201}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="52">
   <si>
     <t>Name</t>
   </si>
@@ -192,6 +192,12 @@
   <si>
     <t>Murali(USGI51340704)
 Rajalaxmi(USGI53042804)</t>
+  </si>
+  <si>
+    <t>25th JAN 2026</t>
+  </si>
+  <si>
+    <t>K3220367</t>
   </si>
 </sst>
 </file>
@@ -343,9 +349,6 @@
     <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -353,6 +356,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -374,9 +380,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -414,7 +420,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -520,7 +526,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -662,7 +668,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -672,8 +678,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5689222B-D505-40C9-8681-40BFCA167C6B}">
   <dimension ref="A1:N18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -807,13 +813,13 @@
       <c r="I3" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="J3" s="21" t="s">
+      <c r="J3" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="K3" s="22" t="s">
+      <c r="K3" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="L3" s="23" t="s">
+      <c r="L3" s="22" t="s">
         <v>39</v>
       </c>
       <c r="M3" s="19">
@@ -950,7 +956,9 @@
       <c r="B10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="1"/>
+      <c r="C10" s="1" t="s">
+        <v>51</v>
+      </c>
       <c r="D10" s="1" t="s">
         <v>17</v>
       </c>
@@ -969,8 +977,12 @@
       <c r="I10" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
+      <c r="J10" s="8">
+        <v>46009</v>
+      </c>
+      <c r="K10" s="8">
+        <v>65368</v>
+      </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
@@ -979,14 +991,18 @@
       <c r="B11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="1"/>
+      <c r="C11" s="1">
+        <v>170557110</v>
+      </c>
       <c r="D11" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F11" s="1"/>
+      <c r="F11" s="1" t="s">
+        <v>50</v>
+      </c>
       <c r="G11" s="4" t="s">
         <v>26</v>
       </c>
@@ -996,30 +1012,34 @@
       <c r="I11" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
+      <c r="J11" s="8">
+        <v>21210</v>
+      </c>
+      <c r="K11" s="8">
+        <v>58101</v>
+      </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A17" s="20" t="s">
+      <c r="A17" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="B17" s="20"/>
-      <c r="C17" s="20"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="20"/>
-      <c r="G17" s="20"/>
-      <c r="H17" s="20"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="23"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="23"/>
+      <c r="G17" s="23"/>
+      <c r="H17" s="23"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A18" s="20"/>
-      <c r="B18" s="20"/>
-      <c r="C18" s="20"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="20"/>
-      <c r="F18" s="20"/>
-      <c r="G18" s="20"/>
-      <c r="H18" s="20"/>
+      <c r="A18" s="23"/>
+      <c r="B18" s="23"/>
+      <c r="C18" s="23"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="23"/>
+      <c r="G18" s="23"/>
+      <c r="H18" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>